<commit_message>
changed one shoot length in growth shoot data
</commit_message>
<xml_diff>
--- a/biol402_growth_shoot_data.xlsx
+++ b/biol402_growth_shoot_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maryo/GitHub/biol_402/Biol_402_2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E475FE1-C213-9F43-8A7A-04195CDFFDF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07EF0E59-CF2F-B342-A6E5-3739D79B2E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15440" xr2:uid="{26387827-D6A3-914C-9F8E-DD946CED528D}"/>
   </bookViews>
@@ -660,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB2678D1-3612-2E43-9A51-B3B7B8EAB60E}">
   <dimension ref="A1:BM70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57:XFD60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6074,8 +6074,8 @@
       <c r="G39" s="1">
         <v>11</v>
       </c>
-      <c r="H39" s="1">
-        <v>75.3</v>
+      <c r="H39" s="12">
+        <v>109.4</v>
       </c>
       <c r="I39" s="1">
         <v>0.6</v>

</xml_diff>

<commit_message>
revised a point on the shoot growth data
</commit_message>
<xml_diff>
--- a/biol402_growth_shoot_data.xlsx
+++ b/biol402_growth_shoot_data.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maryo/GitHub/biol_402/Biol_402_2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07EF0E59-CF2F-B342-A6E5-3739D79B2E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F34A70B-4729-1547-8DBE-9F5075751FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15440" xr2:uid="{26387827-D6A3-914C-9F8E-DD946CED528D}"/>
+    <workbookView xWindow="780" yWindow="1000" windowWidth="19040" windowHeight="12000" xr2:uid="{26387827-D6A3-914C-9F8E-DD946CED528D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -257,7 +257,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -299,6 +299,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -320,7 +327,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -344,6 +351,7 @@
     </xf>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -660,7 +668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB2678D1-3612-2E43-9A51-B3B7B8EAB60E}">
   <dimension ref="A1:BM70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
       <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
@@ -4938,8 +4946,9 @@
       <c r="G31" s="1">
         <v>11</v>
       </c>
-      <c r="H31" s="1">
-        <v>81.2</v>
+      <c r="H31" s="12">
+        <f>81.2+23.5</f>
+        <v>104.7</v>
       </c>
       <c r="I31" s="1">
         <v>0.7</v>
@@ -7898,7 +7907,7 @@
       <c r="I51" s="1">
         <v>0.5</v>
       </c>
-      <c r="J51" s="1">
+      <c r="J51" s="13">
         <v>58.5</v>
       </c>
       <c r="K51" s="1">

</xml_diff>